<commit_message>
Release(02.11.2022 0:11): Refactoring release
</commit_message>
<xml_diff>
--- a/Работа/2. Отчеты/1. Ежедневный/4. Простои и сервис/2022/09. Сентябрь/!!! Рейтинги_Сентябрь 2022.xlsx
+++ b/Работа/2. Отчеты/1. Ежедневный/4. Простои и сервис/2022/09. Сентябрь/!!! Рейтинги_Сентябрь 2022.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F236DD1-910F-4B10-9EFD-4AA775342D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01.09" sheetId="90" r:id="rId1"/>
@@ -12,8 +13,9 @@
     <sheet name="05.09" sheetId="92" r:id="rId3"/>
     <sheet name="06.09" sheetId="93" r:id="rId4"/>
     <sheet name="07.09" sheetId="94" r:id="rId5"/>
+    <sheet name="08.09" sheetId="95" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -23,6 +25,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="20">
   <si>
     <t>Калининград</t>
   </si>
@@ -87,12 +90,15 @@
   </si>
   <si>
     <t>Рейтинг подразделений по 4 показателям за 07.09.2022</t>
+  </si>
+  <si>
+    <t>Рейтинг подразделений по 4 показателям за 08.09.2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -184,7 +190,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -217,9 +223,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -252,6 +275,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -427,7 +467,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -552,7 +592,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:B16">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B16">
     <sortCondition ref="A3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -560,7 +600,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -687,7 +727,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:B16">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B16">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -695,7 +735,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -814,7 +854,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:B15">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B15">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -822,7 +862,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -939,7 +979,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:B15">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B15">
     <sortCondition ref="A3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -947,7 +987,134 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B15">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5727B9-0051-4CC2-AEF7-6DD4EE1BD7F9}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -958,7 +1125,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1066,8 +1233,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:B15">
-    <sortCondition ref="A1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B15">
+    <sortCondition ref="A3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>